<commit_message>
commit log updated + progress report 2
</commit_message>
<xml_diff>
--- a/commit_log.xlsx
+++ b/commit_log.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\odassa\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\omri\Desktop\project_HUJI\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{6CAD0405-D223-4D3D-BCEE-3CFE52DA4F2C}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17424" windowHeight="9624"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="22">
   <si>
     <t>NAME</t>
   </si>
@@ -36,12 +37,66 @@
   </si>
   <si>
     <t>COMMENT</t>
+  </si>
+  <si>
+    <t>Omri</t>
+  </si>
+  <si>
+    <t>16.12.18</t>
+  </si>
+  <si>
+    <t>address_translation.v</t>
+  </si>
+  <si>
+    <t>Ori</t>
+  </si>
+  <si>
+    <t>cache.v</t>
+  </si>
+  <si>
+    <t>interface created</t>
+  </si>
+  <si>
+    <t>spi.v</t>
+  </si>
+  <si>
+    <t>deleting unnesecery states from state machine</t>
+  </si>
+  <si>
+    <t>interconnect.v</t>
+  </si>
+  <si>
+    <t>adjesting interface according to address_translation.v</t>
+  </si>
+  <si>
+    <t>19.12.18</t>
+  </si>
+  <si>
+    <t>per_home_logic.v</t>
+  </si>
+  <si>
+    <t>cpu_if.v</t>
+  </si>
+  <si>
+    <t>taking down one sample stage for read data</t>
+  </si>
+  <si>
+    <t>23.12.18</t>
+  </si>
+  <si>
+    <t>address_translation4k.v</t>
+  </si>
+  <si>
+    <t>inserting basic translation for spesific case in order to check functionality</t>
+  </si>
+  <si>
+    <t>inserting NVM read request stage to spi state machine</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -91,13 +146,13 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:D44" totalsRowShown="0">
-  <autoFilter ref="A1:D44"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:D44" totalsRowShown="0">
+  <autoFilter ref="A1:D44" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="4">
-    <tableColumn id="1" name="NAME"/>
-    <tableColumn id="2" name="DATE"/>
-    <tableColumn id="3" name="FILE"/>
-    <tableColumn id="4" name="COMMENT"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="NAME"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="DATE"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="FILE"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="COMMENT"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -365,22 +420,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.109375" customWidth="1"/>
-    <col min="2" max="2" width="31.44140625" customWidth="1"/>
-    <col min="3" max="3" width="28.5546875" customWidth="1"/>
-    <col min="4" max="4" width="25.44140625" customWidth="1"/>
+    <col min="1" max="1" width="16.140625" customWidth="1"/>
+    <col min="2" max="2" width="31.42578125" customWidth="1"/>
+    <col min="3" max="3" width="28.5703125" customWidth="1"/>
+    <col min="4" max="4" width="67" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -392,6 +447,118 @@
       </c>
       <c r="D1" t="s">
         <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" t="s">
+        <v>15</v>
+      </c>
+      <c r="D6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" t="s">
+        <v>16</v>
+      </c>
+      <c r="D7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>4</v>
+      </c>
+      <c r="B8" t="s">
+        <v>18</v>
+      </c>
+      <c r="C8" t="s">
+        <v>19</v>
+      </c>
+      <c r="D8" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" t="s">
+        <v>18</v>
+      </c>
+      <c r="C9" t="s">
+        <v>10</v>
+      </c>
+      <c r="D9" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
schems , reports , commits ,readme updated
</commit_message>
<xml_diff>
--- a/commit_log.xlsx
+++ b/commit_log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\omri\Desktop\project_HUJI\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{6CAD0405-D223-4D3D-BCEE-3CFE52DA4F2C}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{8502C889-2CB9-46D4-83F6-8E45BED760E7}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="27">
   <si>
     <t>NAME</t>
   </si>
@@ -91,6 +91,21 @@
   </si>
   <si>
     <t>inserting NVM read request stage to spi state machine</t>
+  </si>
+  <si>
+    <t>2.1.19</t>
+  </si>
+  <si>
+    <t>vf2pf.v</t>
+  </si>
+  <si>
+    <t>selection between regular pf , vf2pf , 4k translation added , shourtcuted to the output</t>
+  </si>
+  <si>
+    <t xml:space="preserve">connecting cache req to nvm read stage in spi state machine </t>
+  </si>
+  <si>
+    <t xml:space="preserve">collect read data from nvm interface </t>
   </si>
 </sst>
 </file>
@@ -421,18 +436,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.140625" customWidth="1"/>
-    <col min="2" max="2" width="31.42578125" customWidth="1"/>
-    <col min="3" max="3" width="28.5703125" customWidth="1"/>
-    <col min="4" max="4" width="67" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="78.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -559,6 +574,62 @@
       </c>
       <c r="D9" t="s">
         <v>21</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>4</v>
+      </c>
+      <c r="B10" t="s">
+        <v>22</v>
+      </c>
+      <c r="C10" t="s">
+        <v>23</v>
+      </c>
+      <c r="D10" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>4</v>
+      </c>
+      <c r="B11" t="s">
+        <v>22</v>
+      </c>
+      <c r="C11" t="s">
+        <v>6</v>
+      </c>
+      <c r="D11" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>7</v>
+      </c>
+      <c r="B12" t="s">
+        <v>22</v>
+      </c>
+      <c r="C12" t="s">
+        <v>10</v>
+      </c>
+      <c r="D12" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>7</v>
+      </c>
+      <c r="B13" t="s">
+        <v>22</v>
+      </c>
+      <c r="C13" t="s">
+        <v>10</v>
+      </c>
+      <c r="D13" t="s">
+        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update all reports + commit log
</commit_message>
<xml_diff>
--- a/commit_log.xlsx
+++ b/commit_log.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\omri\Desktop\project_HUJI\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D42C65C3-BE63-4C35-BE59-4421D8CDBD05}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCDBBDCE-E479-4768-BAE2-5DAE09E3A64E}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="114">
   <si>
     <t>NAME</t>
   </si>
@@ -313,6 +313,60 @@
   </si>
   <si>
     <t>pinning fix - pin action of "NO_ACTION" unpinned a pinned address.</t>
+  </si>
+  <si>
+    <t>14.4.19</t>
+  </si>
+  <si>
+    <t>21.4.19</t>
+  </si>
+  <si>
+    <t>28.4.19</t>
+  </si>
+  <si>
+    <t>19.5.19</t>
+  </si>
+  <si>
+    <t>12.5.19</t>
+  </si>
+  <si>
+    <t>5.5.19</t>
+  </si>
+  <si>
+    <t>advance address protection coded</t>
+  </si>
+  <si>
+    <t>LRU supports partial maping</t>
+  </si>
+  <si>
+    <t>MISS HANDLER support partial mapping</t>
+  </si>
+  <si>
+    <t>FIXing lintra problems</t>
+  </si>
+  <si>
+    <t>all files</t>
+  </si>
+  <si>
+    <t>Mapping testbanch</t>
+  </si>
+  <si>
+    <t>all cache</t>
+  </si>
+  <si>
+    <t>PROTECTION testbanch</t>
+  </si>
+  <si>
+    <t>all AT</t>
+  </si>
+  <si>
+    <t>code coverage and tools cleaning</t>
+  </si>
+  <si>
+    <t>establishing rules for Formal varification</t>
+  </si>
+  <si>
+    <t>Debug formal varification fails</t>
   </si>
 </sst>
 </file>
@@ -643,10 +697,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D53"/>
+  <dimension ref="A1:D65"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D43" sqref="D43"/>
+    <sheetView tabSelected="1" topLeftCell="A51" workbookViewId="0">
+      <selection activeCell="D66" sqref="D66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1399,6 +1453,174 @@
         <v>81</v>
       </c>
     </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>4</v>
+      </c>
+      <c r="B54" t="s">
+        <v>96</v>
+      </c>
+      <c r="C54" t="s">
+        <v>6</v>
+      </c>
+      <c r="D54" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>7</v>
+      </c>
+      <c r="B55" t="s">
+        <v>96</v>
+      </c>
+      <c r="C55" t="s">
+        <v>37</v>
+      </c>
+      <c r="D55" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>7</v>
+      </c>
+      <c r="B56" t="s">
+        <v>97</v>
+      </c>
+      <c r="C56" t="s">
+        <v>35</v>
+      </c>
+      <c r="D56" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>4</v>
+      </c>
+      <c r="B57" t="s">
+        <v>97</v>
+      </c>
+      <c r="C57" t="s">
+        <v>106</v>
+      </c>
+      <c r="D57" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>7</v>
+      </c>
+      <c r="B58" t="s">
+        <v>98</v>
+      </c>
+      <c r="C58" t="s">
+        <v>108</v>
+      </c>
+      <c r="D58" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>4</v>
+      </c>
+      <c r="B59" t="s">
+        <v>98</v>
+      </c>
+      <c r="C59" t="s">
+        <v>110</v>
+      </c>
+      <c r="D59" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>7</v>
+      </c>
+      <c r="B60" t="s">
+        <v>101</v>
+      </c>
+      <c r="C60" t="s">
+        <v>106</v>
+      </c>
+      <c r="D60" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>4</v>
+      </c>
+      <c r="B61" t="s">
+        <v>101</v>
+      </c>
+      <c r="C61" t="s">
+        <v>106</v>
+      </c>
+      <c r="D61" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>7</v>
+      </c>
+      <c r="B62" t="s">
+        <v>100</v>
+      </c>
+      <c r="C62" t="s">
+        <v>106</v>
+      </c>
+      <c r="D62" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>4</v>
+      </c>
+      <c r="B63" t="s">
+        <v>100</v>
+      </c>
+      <c r="C63" t="s">
+        <v>106</v>
+      </c>
+      <c r="D63" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>7</v>
+      </c>
+      <c r="B64" t="s">
+        <v>99</v>
+      </c>
+      <c r="C64" t="s">
+        <v>106</v>
+      </c>
+      <c r="D64" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>4</v>
+      </c>
+      <c r="B65" t="s">
+        <v>99</v>
+      </c>
+      <c r="C65" t="s">
+        <v>106</v>
+      </c>
+      <c r="D65" t="s">
+        <v>113</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">

</xml_diff>